<commit_message>
I have added some of my unit tests and updated the regression test
</commit_message>
<xml_diff>
--- a/RegressionTest.xlsx
+++ b/RegressionTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\cs5101\RAAY-connect4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\aaa\gitrepo\RAAY-connect4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Pass / Fail</t>
   </si>
@@ -51,6 +51,24 @@
   </si>
   <si>
     <t>TestController:test sendstringmessage() by declaring a string and compare with output of sendstringmessage()</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>completing a horizontal set of 4. The AI sets a 2 on the right of this group.</t>
+  </si>
+  <si>
+    <t>AIVerticalTest1(): This test sets up the board in such a manner that the AI opponent places a 2 on any stack of 3 1's that the human player places.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIHorizontalTest1(): This test sets up the board in a manner such that the AI opponent places a piece to prevent the human player from winning by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIDiagonalRightTest1(): This test sets up the board in such a manner that the AI opponent places a 2 on a group of 1's that form a "right diagonal". </t>
+  </si>
+  <si>
+    <t>AIDiagonalLeftTest1(): This test sets up the board in such a manner that the AI opponent places a 2 on a group of 1's that form a "left diagonal".</t>
   </si>
 </sst>
 </file>
@@ -383,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -442,6 +460,43 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
have included all of my unit tests that I have used through the project  and updated the regression test accordingly.
</commit_message>
<xml_diff>
--- a/RegressionTest.xlsx
+++ b/RegressionTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\aaa\gitrepo\RAAY-connect4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Desktop\class crap\QA\connect4\RAAY-connect4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Pass / Fail</t>
   </si>
@@ -69,6 +72,18 @@
   </si>
   <si>
     <t>AIDiagonalLeftTest1(): This test sets up the board in such a manner that the AI opponent places a 2 on a group of 1's that form a "left diagonal".</t>
+  </si>
+  <si>
+    <t>AIHolesTest1(): This test sets up the board in such a manner that the AI places a 2 into the hole in the 1's.</t>
+  </si>
+  <si>
+    <t>AILeft2Test1(): This test sets up the board and tests the AI's left-of-the-group placement.</t>
+  </si>
+  <si>
+    <t>AIRight2Test1(): This test sets up the board and tests the AI's right-of-the-group placement.</t>
+  </si>
+  <si>
+    <t>AITop2Test1(): This test sets up the board and tests the AI's vertical placement.</t>
   </si>
 </sst>
 </file>
@@ -125,8 +140,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -401,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -497,6 +540,38 @@
         <v>9</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>